<commit_message>
failed attempts to calibrate emissions
</commit_message>
<xml_diff>
--- a/Data/cleaned_and_combined_data/Carbon_Intensity/Carbon_Intensity_Constants.xlsx
+++ b/Data/cleaned_and_combined_data/Carbon_Intensity/Carbon_Intensity_Constants.xlsx
@@ -15,7 +15,20 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -92,6 +105,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -140,16 +154,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,7 +468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B55" sqref="B55:E57"/>
     </sheetView>
   </sheetViews>
@@ -478,802 +492,802 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="5">
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3">
         <v>149.30000000000001</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="3">
         <v>80.599999999999994</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="5">
+      <c r="A3" s="5"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3">
         <v>187.8</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <v>59.4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5">
+      <c r="A4" s="5"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3">
         <v>7.2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="5">
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3">
         <v>159.30000000000001</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>84.7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="5">
+      <c r="A6" s="5"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3">
         <v>195.1</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="3">
         <v>61.1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5">
+      <c r="A7" s="5"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3">
         <v>0.8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="5"/>
+      <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="5">
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3">
         <v>135</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="3">
         <v>90.3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="5">
+      <c r="A9" s="5"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3">
         <v>137.9</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="3">
         <v>88.7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="5">
+      <c r="A10" s="5"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3">
         <v>106.3</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="3">
         <v>13.1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="5">
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3">
         <v>149</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="3">
         <v>80.400000000000006</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="5">
+      <c r="A12" s="5"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="3">
         <v>200.6</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="3">
         <v>62.3</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5">
+      <c r="A13" s="5"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3">
         <v>7.2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3" t="s">
+      <c r="A14" s="5"/>
+      <c r="B14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="5">
+      <c r="C14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="3">
         <v>135.19999999999999</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="3">
         <v>74.2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="5">
+      <c r="A15" s="5"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="3">
         <v>169.9</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="3">
         <v>55.5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5">
+      <c r="A16" s="5"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3">
         <v>0.25</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3" t="s">
+      <c r="A17" s="5"/>
+      <c r="B17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="5">
+      <c r="C17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="3">
         <v>138.69999999999999</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="3">
         <v>101.9</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="2"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="5">
+      <c r="A18" s="5"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="3">
         <v>165.4</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="3">
         <v>52.4</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="2"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5">
+      <c r="A19" s="5"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3">
         <v>27.9</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="5">
+      <c r="C20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="3">
         <v>138.69999999999999</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="3">
         <v>74.3</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="5">
+      <c r="A21" s="5"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="3">
         <v>165.4</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="3">
         <v>54.8</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="2"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5">
+      <c r="A22" s="5"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3">
         <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="2"/>
-      <c r="B23" s="3" t="s">
+      <c r="A23" s="5"/>
+      <c r="B23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="5">
+      <c r="C23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="3">
         <v>135.19999999999999</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="3">
         <v>74.2</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="2"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="5">
+      <c r="A24" s="5"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="3">
         <v>168.2</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="3">
         <v>55.1</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="2"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5">
+      <c r="A25" s="5"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3">
         <v>1.2</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="2"/>
-      <c r="B26" s="3" t="s">
+      <c r="A26" s="5"/>
+      <c r="B26" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="5">
+      <c r="C26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="3">
         <v>136.5</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="3">
         <v>103.4</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="2"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="5">
+      <c r="A27" s="5"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="3">
         <v>129</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27" s="3">
         <v>88.3</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="2"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5">
+      <c r="A28" s="5"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3">
         <v>11.4</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="5">
+      <c r="C29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="3">
         <v>148.9</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29" s="3">
         <v>80.7</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="2"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="5">
+      <c r="A30" s="5"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="3">
         <v>199</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30" s="3">
         <v>62.5</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="2"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5">
+      <c r="A31" s="5"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3">
         <v>7.2</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="2"/>
-      <c r="B32" s="3" t="s">
+      <c r="A32" s="5"/>
+      <c r="B32" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" s="5">
+      <c r="C32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="3">
         <v>135.9</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32" s="3">
         <v>76.400000000000006</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="2"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" s="5">
+      <c r="A33" s="5"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="3">
         <v>157.9</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E33" s="3">
         <v>53.3</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="2"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5">
+      <c r="A34" s="5"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3">
         <v>0.3</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="2"/>
-      <c r="B35" s="3" t="s">
+      <c r="A35" s="5"/>
+      <c r="B35" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" s="5">
+      <c r="C35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="3">
         <v>127.1</v>
       </c>
-      <c r="E35" s="5">
+      <c r="E35" s="3">
         <v>99.5</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="2"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" s="5">
+      <c r="A36" s="5"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="3">
         <v>129.1</v>
       </c>
-      <c r="E36" s="5">
+      <c r="E36" s="3">
         <v>88.3</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="2"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5">
+      <c r="A37" s="5"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3">
         <v>12.1</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" s="5">
+      <c r="C38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="3">
         <v>144.6</v>
       </c>
-      <c r="E38" s="5">
+      <c r="E38" s="3">
         <v>89.8</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="2"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="5">
+      <c r="A39" s="5"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="3">
         <v>162.6</v>
       </c>
-      <c r="E39" s="5">
+      <c r="E39" s="3">
         <v>54.4</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="2"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5">
+      <c r="A40" s="5"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3">
         <v>-4.9000000000000004</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="2"/>
-      <c r="B41" s="3" t="s">
+      <c r="A41" s="5"/>
+      <c r="B41" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
+      <c r="C41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="2"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" s="5">
+      <c r="A42" s="5"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="3">
         <v>145.19999999999999</v>
       </c>
-      <c r="E42" s="5">
+      <c r="E42" s="3">
         <v>89.9</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="2"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D43" s="5">
+      <c r="A43" s="5"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="3">
         <v>157.30000000000001</v>
       </c>
-      <c r="E43" s="5">
+      <c r="E43" s="3">
         <v>53.2</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="2"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5">
+      <c r="A44" s="5"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3">
         <v>1.7</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="2"/>
-      <c r="B45" s="3" t="s">
+      <c r="A45" s="5"/>
+      <c r="B45" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
+      <c r="C45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="2"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" s="5">
+      <c r="A46" s="5"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="3">
         <v>130.30000000000001</v>
       </c>
-      <c r="E46" s="5">
+      <c r="E46" s="3">
         <v>100.9</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="2"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D47" s="5">
+      <c r="A47" s="5"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="3">
         <v>128.5</v>
       </c>
-      <c r="E47" s="5">
+      <c r="E47" s="3">
         <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="2"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5">
+      <c r="A48" s="5"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3">
         <v>11.9</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5">
+      <c r="C49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3">
         <v>50.5</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="2"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5">
+      <c r="A50" s="5"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3">
         <v>39.9</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="2"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5">
+      <c r="A51" s="5"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3">
         <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" s="2"/>
-      <c r="B52" s="3" t="s">
+      <c r="A52" s="5"/>
+      <c r="B52" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5">
+      <c r="C52" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3">
         <v>80.400000000000006</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53" s="2"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5">
+      <c r="A53" s="5"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3">
         <v>45.2</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="2"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5">
+      <c r="A54" s="5"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="2"/>
-      <c r="B55" s="3" t="s">
+      <c r="A55" s="5"/>
+      <c r="B55" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C55" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5">
+      <c r="C55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3">
         <v>69.8</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" s="2"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5">
+      <c r="A56" s="5"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3">
         <v>40.799999999999997</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="2"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5">
+      <c r="A57" s="5"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3">
         <v>6.7</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C58" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5">
+      <c r="C58" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3">
         <v>61.9</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" s="2"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5">
+      <c r="A59" s="5"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3">
         <v>29.4</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" s="2"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5">
+      <c r="A60" s="5"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3">
         <v>-6.7</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" s="2"/>
-      <c r="B61" s="3" t="s">
+      <c r="A61" s="5"/>
+      <c r="B61" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C61" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5">
+      <c r="C61" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3">
         <v>63.4</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="2"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5">
+      <c r="A62" s="5"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3">
         <v>29.7</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63" s="2"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5">
+      <c r="A63" s="5"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3">
         <v>-6.4</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" s="2"/>
-      <c r="B64" s="2" t="s">
+      <c r="A64" s="5"/>
+      <c r="B64" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C64" s="1" t="s">
@@ -1284,8 +1298,8 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65" s="2"/>
-      <c r="B65" s="2"/>
+      <c r="A65" s="5"/>
+      <c r="B65" s="5"/>
       <c r="C65" s="1" t="s">
         <v>8</v>
       </c>
@@ -1294,8 +1308,8 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66" s="2"/>
-      <c r="B66" s="2"/>
+      <c r="A66" s="5"/>
+      <c r="B66" s="5"/>
       <c r="C66" s="1" t="s">
         <v>9</v>
       </c>
@@ -1305,13 +1319,11 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="B52:B54"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A11:A19"/>
+    <mergeCell ref="A20:A28"/>
+    <mergeCell ref="A29:A37"/>
+    <mergeCell ref="A38:A48"/>
     <mergeCell ref="A49:A57"/>
     <mergeCell ref="A58:A66"/>
     <mergeCell ref="B2:B4"/>
@@ -1328,11 +1340,13 @@
     <mergeCell ref="B35:B37"/>
     <mergeCell ref="B38:B40"/>
     <mergeCell ref="B41:B44"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="A11:A19"/>
-    <mergeCell ref="A20:A28"/>
-    <mergeCell ref="A29:A37"/>
-    <mergeCell ref="A38:A48"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="B58:B60"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>